<commit_message>
Get daily reddit data: Tue May 27 08:12:36 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_01.xlsx
+++ b/data/collected_data/2025_06_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C508"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3525 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1kwhk0q</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>What to ask to have fixed?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwhk0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1kwhbx8</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>struggling with gel nail longevity</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlp8xv0d2a3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1kwh4fp</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Did em without tools🤧</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnjow0xrz93f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1kwgu5k</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Nail art</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pd50rsbw93f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1kwg49d</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Best manicure I’ve received</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k02vahvmn93f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1kwg3ic</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Nail ideas</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v22vcl5en93f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1kwg0xc</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2706i6gkm93f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1kwfadt</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>gel x</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwfadt/gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1kwf5k1</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Soft or hard gel builder manicure for brittle/easy bending nails?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwf5k1/soft_or_hard_gel_builder_manicure_for_brittleeasy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1kwejak</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>New press ons!!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwejak</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1kwedcv</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>This years pride nails 🌈</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3c7qybx9493f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1kwbmdf</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>salon fix for split nail?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7i0sepnd83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1kwcdjv</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Began my natural nail journey. How do i keep them white, shiny, and strong?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwcdjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1kwb09z</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Butterfly Nails! 🦋</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwb09z</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1kwdxbr</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Nails for my wedding</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwdxbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1kwduq1</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Purple Chrome Butterfly 🦋</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwduq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1kwdpo0</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Brown 🧸🍫</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gpxhjzkx83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1kwctf5</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Pride nails ✨🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g82ibghqo83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1kwcouj</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>First time doing at home dip powder</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwcouj</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1kwchay</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Nail supply websites</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwchay/nail_supply_websites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1kwchax</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Rate my nails 🌸</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwchax</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1kwccv2</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>My nail growth after 3 weeks</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwccv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1kwcc20</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Still can’t use EDJY properly</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwcc20/still_cant_use_edjy_properly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1kwbx8v</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Idk if I like them🥲😂</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgbglmucg83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1kwbhs4</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>First attempt at a marble effect- how did I do?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jr5nc9qfc83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1kwbgeo</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>First time getting nails done, how do they look?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwbgeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1kwbfmo</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Strawberry picnic nails for spring! 🍓</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdhdtejwb83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1kwbelx</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>The set I made for this week. Not sure if I like it or not ...</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwbelx</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1kwb2un</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dob0spcm883f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1kwaw6r</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Central Texas nail artists</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwaw6r/central_texas_nail_artists/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1kwag5i</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Went Back to My Nail Tech… He Did Not Disappoint!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwag5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1kwan3u</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>attempt with gel polish</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21app79k483f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1kwadmj</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Atomic Polish’s Violet Flame (August ‘21 PPU)</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwadmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1kwabzc</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Color regret?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwabzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1kw9zmv</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Birthday Nails - UV gel extensions</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50y7cb6my73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1kw9xb7</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>which shape looks better ?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw9xb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1kw9ulo</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>First acrylic-chose "squoval" shape-does it suit my hands?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw9ulo</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1kw9os0</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Ocean nails~ 🐟</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw9os0</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1kw9ksw</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Are these cute? I’ve been doing my nails at home for about a year. I’m not super creative so idkkk</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t554f2hvu73f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1kw9ee2</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Best mani of my life for Palm Springs!</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw9ee2</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1kw96hr</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Builder gel nails 💕</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvuumfodr73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1kw964e</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>How to keep my nails from breaking off after removing acrylics?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw964e/how_to_keep_my_nails_from_breaking_off_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1kw93qg</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>First acrylic set on a real hand 🖐️</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e40vtshpq73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1kw8zvw</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Tropical vibes</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z688kjesp73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1kw8y8l</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>I don’t have much I can do in way of painting my own nails right now, but these are a few ideas I have for nail art goals. What do you think? 🤔</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw8y8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1kw8vrx</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Some of the mani/pedis I’ve had over the years</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw8vrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1kw8s8e</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>4 hours later and I’m finished!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw8s8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1kw8l3g</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>How much would you say this set is worth?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93tg67e2m73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1kw8fi3</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Found online and they are sooo cute 🐞</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtnhivzwk73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1kw8esk</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Beginner nail art</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr48rttqk73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1kw89vf</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Couples Mani 💧Feat. Finger Creeper Pose 🤣</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw89vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1kw790p</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>⚠️WARNING! DO NOT USE GLAMNETIC! ⚠️</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwlc67jcb73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1kw7wkg</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Pool party vibes for my Russian mani</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw7wkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1kw7sop</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Acrylic removal 😭</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw7sop/acrylic_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1kw7ojj</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Tiny short nailbeds</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56uek10re73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1kw7jpi</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Have I filed my side walls too much? Or is my shaping bad for my nails</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw7jpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1kw74dv</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Nail Stencil Tips?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lbhoo1ca73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1kw6yax</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Summer set with gelx</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9bhyqk0973f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1kw6aqo</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Should I get my nails redone even if it’s been less than 2 weeks?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptdlbduy373f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1kw65xy</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Small crack</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw65xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1kw6507</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Male interested in nail art</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw6507/male_interested_in_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1kw5ihl</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Why is my nail polish taking hours to dry?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw5ihl/why_is_my_nail_polish_taking_hours_to_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1kw5o35</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>New independent nail tech I found 🥰 $65 Oklahoma</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw5o35</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1kw5maq</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Which shape looks better on me?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw5maq</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1kw565v</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Gel nails getting bumps/bubbles a week after getting them done!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw565v</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1kw4v0q</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Pre-painted Nail Tips?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw4v0q/prepainted_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1kw4j9w</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Do you like my new design? 💙</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9d220mvq63f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1kw4j2g</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Little limes</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hplv85vtq63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1kw4a9f</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Nails were Long and Strong 6 Months Ago</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw4a9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1kw3rsp</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Lemon holiday nails</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnh1l548l63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1kw336h</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>not a big fan of pink alone,what do y’all think?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k7n2qdx1g63f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1kvz53g</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Please help with curved nails!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvz53g</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1kvzs0s</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Can I put an acrylic back on this?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvzs0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1kw0xvt</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>How to remove biab with tips without damaging already weak nails?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9em556r063f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1kw2uxz</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Snakes &amp; flowers🐍🌸</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tsk7zp7fe63f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1kvxw7d</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Slowly trying to get back into nail art</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/653g95c4f53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1kw2r3r</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>I went with the stilettos. I love them!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1o1prfand63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1kw2fw4</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>No more gels</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw2fw4/no_more_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1kw2hlo</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Used jewellery glue</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw2hlo/used_jewellery_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1kw1e03</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Is it me or something else?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw1e03/is_it_me_or_something_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1kw171e</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Nail tech over filed my nail beds before applying gel polish.. need advice please!</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfpv8zqi263f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1kw28rv</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Periwinkle French tips with sparkles for EDC Vegas last weekend</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btopvlr1a63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1kw0qqq</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Nail split? After taking off press on</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cw1e2uwcz53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1kw1tvt</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Should I stop going to my nail salon?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cong8r22763f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1kw1sqf</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Polish that looks natural?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw1sqf/polish_that_looks_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1kw1kbj</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Fresh Dip!</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8jlnp46563f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1kw17so</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Rings of fire?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qg1a1zn263f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1kw17av</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Best nails for newborn moms?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw17av/best_nails_for_newborn_moms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1kw0vy0</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>How to find good nail tech?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kw0vy0/how_to_find_good_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1kw0vek</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Grad party set I did on myself 😊</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw0vek</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1kw074x</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>First time using solid nail glue</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw074x</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1kw064y</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Summer vibes</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw064y</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1kvzvrt</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Non-drying polish remover?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kvzvrt/nondrying_polish_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1kvzo14</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>My beautiful babes</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvzo14</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1kvzcc5</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>I loved this set</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsn27jtgp53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1kvyy48</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Teal mani 🩵</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3moulweom53f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1kvy490</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Cotton Candy?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvy490</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1kvxswq</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Rainbow-like nails</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jvav3ruee53f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1kvqm4o</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Too flat?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvqm4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1kvxey8</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>nail growth update…. a little chippy but 🤷🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nt6elbzlb53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1kwhgxy</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>First attempt at a French tip</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq6np4o44a3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1kwgyiw</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Fun With Magnetics!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwgyiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1kwenbb</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Lacquer 22 Guts or dupe</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwenbb/lacquer_22_guts_or_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1kweez8</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Polished For Days Blossom</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kweez8</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1kwddam</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Finally! An orange I can wear 🦋</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d90iztb3u83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1kwd5wf</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>ILNP Glory vs Holo Taco Fallen Flake Taco?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwd5wf/ilnp_glory_vs_holo_taco_fallen_flake_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1kwcxtw</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>$1.98 LA Colors Metal Finish🪩</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwcxtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1kwaq5z</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Worth the hype</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8kdb1cw283f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1kwaoep</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Yk it’s summer when the neons roll out</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwaoep</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1kw9tf3</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Looking for a Particular Purple</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txuzznf1x73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1kw9p1v</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>LA colors does it again 💕</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw9p1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1kw8z92</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Mango Season ~ orange aura nails</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydieb2vmp73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1kw02po</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>I normally don't post, but I'm kinda proud of this one</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddd8nksju53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1kw6uk3</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Help!!?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw6uk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1kw7sx2</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>What’s Up Beauty 25% off sale ends tonight</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79k6ki4rf73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1kw7fg1</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Who’s copying who??</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw7fg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1kw7a75</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>ILNP strawberry shake: IRL photo vs swatch photo (no drama, just a heads up)</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw7a75</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1kw6d9x</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Medium neutral/olives, what are your favorite pink polishes?</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kw6d9x/medium_neutralolives_what_are_your_favorite_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1kw6a5k</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Greetings Reddit Laqueristas! - Help Needed</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw6a5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1kw5zk7</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>the perfect brown crème</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw5zk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1kw5zg2</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Broken nail what to do 😭</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rd3v9m3l173f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1kw5yt9</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>brown and gold cow print for cowboy carter 🤠</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw5yt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1kw58oj</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Gel nails getting bumps/bubbles a week after getting them done!</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw565v</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1kw4xln</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Still fashionable with a broken arm 🥲</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dn8ht7st63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1kw4xhh</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>I finally tried nail art</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw4xhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1kw4nnq</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhmwt8rkr63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1kw4k99</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Using up DVN: KEROSENE + ROBIN'S EGG</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw4k99</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1kw4in1</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>travelling with polish - case recommendations</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t05lo6rq63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1kw4fh7</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Ofc my PPU arrives after finishing my mani 🙂🙂🙂</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw4fh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1kw4ctb</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Basecoat Battle: oooohhhhoo we’re halfway there…ooohhhooo lemon apple chair!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw4ctb</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1kw4cnn</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Honoring today with some red, white, and blue ❤️🤍💙</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw4cnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1kw3zd5</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>How to make it last</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kw3zd5/how_to_make_it_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1kw351t</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Hard to show the color, but it is really pretty! My first Lurid Lacquer buy!</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wko0fckig63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1kw2yny</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>✨️🌈Minecraft Potion Swatches[*PR*]🌈✨️</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw2yny</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1kw2to0</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Why don’t nail salons practice healthy nail care?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kw2to0/why_dont_nail_salons_practice_healthy_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1kw2ox0</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Neon + Neon = extra Neon!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw2ox0</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1kw284q</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>This shade feels perfect for summer!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw284q</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1kw1q5h</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Swamp Witch deliciousness</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw1q5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1kw1bir</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>The first two pics are swatches of the same polish. I also swatched it in the third picture. Which one (a, b or c) do you think is the polish I received?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw1bir</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1kw1401</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Unacceptable + Soul Sucker 🍋</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw1401</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1kw0pnx</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>I finally got new storage for my nail polishes!</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw0pnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1kvzhpq</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>My Collection!</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73jgsy88q53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1kvzfrp</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Swimming pool blue</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3xax6j4q53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1kvzcq0</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Bit dinged up but here's my mani with a view</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ig9q6igcp53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1kvz1is</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Pheonix indie Daddy kills people 🎂</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvz1is</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1kvyt4g</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Looking for juicy berry red/pink like this</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fmwqgfnl53f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1kvyhrw</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>OPI Koala Bear-y!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8yrmeocj53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1kvybwf</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>this polish has a perfect name…</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvybwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1kvy0v9</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Non drugstore brands that don’t have huge shipping cost or are available in store?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a5om3yj1g53f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1kvxb4h</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Unexpected combo works well together</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0kpz8r5ua53f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1kvwsvt</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Must-have shades from Emily de Molly?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvwsvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1kvwmdk</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>i found a oldie but goodie 😭</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvwmdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1kvw9r4</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Recommendations?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khcjub1a353f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1kvvuut</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Not a skittle fan 😭</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4nlv0v5053f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1kvvqvi</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>What else do I need?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvvqvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1kvuz62</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>messy green skittle! yay!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvuz62</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1kvurs8</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>DIY Jelly with Alcohol Inks and Clear Lacquer</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vulkoh91s43f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1kvudql</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child vs EdM Lament</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kvudql/ilnp_flower_child_vs_edm_lament/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1kvtpb4</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Creme Bundle/Collection Recommendations?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kvtpb4/creme_bundlecollection_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1kvtgrk</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Serpents Of Styx</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4vfzwmb6h43f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1kvt0kd</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>I’m firmly on the Lurid train…</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvt0kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1kvsg5o</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Free gift from Cracked Polish</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvsg5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1kvs5nv</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Cadillacquer - Lunar Eclipse</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvs5nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1kvqobl</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kvqobl/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1kvpthe</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Gold glitter mani</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdaw0chcd33f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1kwe8c7</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Excuse my ring finger nail, it’s growing back after being slammed in kitchen window this summer and 3 stitches later. Nails done by me thooo!JMB(Jean Michel Basquiat)🤴🏾👑🧑🏾‍🎨</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nm8ugfs293f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1kwdb6y</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Grrrr🙊😼💋👜💄💅🏻💅🏻🫦🌙🩷</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7dbhxiit83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1kwchl6</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Every nail design is a new adventure, and I’m just getting started! 🔥 Who’s coming along for the ride?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3b3wjaml83f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1kwcf6w</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Nail supply websites</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kwcf6w/nail_supply_websites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1kwblgx</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>How much do you usually spend on nails?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwblgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1kwbede</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Water colours  or</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/HQp9Q2G.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1kwal70</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>How did I do? Inspo is first pic</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwal70</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1kwakva</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>How did I do? Inspo is first pic</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwakva</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1kw9f99</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>newest set!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed3rjzgjt73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1kw8t9g</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>They took me 4 hours 💛</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw8t9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1kw7z57</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Where on earth do you ladies get your nail charms ??</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kw7z57/where_on_earth_do_you_ladies_get_your_nail_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1kw7y8a</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Alien Theme</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kw7y8a/alien_theme/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1kw7uqc</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Basic and cute</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tplh03ngf73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1kw7rwk</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Unicorn chrome over cats eye</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cp3j55rhf73f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1kw7lzt</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>a little bit of my beautiful work💋</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54p2zh17e73f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1kw6ic5</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>First time trying 3d nail art</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw6ic5</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1kw3wo4</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>El mimo más lindo del día 😍</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw3wo4</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1kw3tb9</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>So proud of these!! Would love feedback!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5dtbfxjl63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1kw3k17</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>My first set since Feburary!!! So happy to be back in the swing of things</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw3k17</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1kw375d</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>When I first started out in nail school 😭</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16zza0lyg63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1kw34xr</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Simple but cute 🧡☺️</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icodklwhg63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1kw2rbr</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Feeling Regal today</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/176rlk5qd63f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1kw2fru</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Medieval inspired ♥️🗡️</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw2fru</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1kw025s</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Summer vibes</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kw025s</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1kvyzj2</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>saw a new technique on this sub the other day so ty :)</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvyzj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1kvyrta</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>What’s your favorite scary movie?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30seisvdl53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1kvy3u6</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I was watching Nail Sesh on tiktok yesterday and they made flowers using nail ink, I wanted to try. Not too bad</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvfjy2amg53f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1kvvg6t</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Las one I promise lol! Nails done by muah!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51bq8db4x43f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1kvvfam</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Nails done by muah!</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3phhswxw43f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1kvve4v</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Nails done by me! Found my sister nail polish and kits!</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l80vviipw43f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1kvvcj7</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Nails done by muah! It’s cool that my sister lets me use her nail polish and kits!</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j56qmn9ew43f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1kvvb1x</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Nails done by muah! Blue and gold my fav colors.</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64uufgg3w43f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1kvurhc</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Gucci Gang! Nails and gem work all done by muah!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5p2hbv5zr43f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1kvup0j</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>A lil Burberry moment!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ctkt8ver43f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1kvt34w</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Mi set favorito por indigonails</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvt34w</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1kvrz9j</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Hand painted Minnie and Mickey in preparation for starting a nail art TikTok!</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvrz9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1kvqsff</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Basquiat🤴🏾Nails done by me!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4tk99cbp33f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1kvqr7u</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Nails done by me! OTM(Nicki) JMB(Basquiat)</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvqr7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1kvqplj</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>I do my own nails! 💕🦄🎀NM</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvqplj</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1kvqo72</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Homage to my 2 favs! Nicki Minaj and Jean Michel Basquiat!👸🏾🤴🏾💅🏾</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvqo72</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1kvqmw9</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Talk to me nice, I’m a beginner nail painter!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kvqmw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1kvp9a8</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>rave nail set!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uxgcv3g633f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May 28 08:12:43 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_01.xlsx
+++ b/data/collected_data/2025_06_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C508"/>
+  <dimension ref="A1:C716"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9069,6 +9069,3542 @@
         </is>
       </c>
     </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1kxb7ag</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Strawberry nails</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxb7ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1kxb77t</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Builder gel refill ♡ + CURSED POSE</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxb77t</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1kxb0ac</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Soft and cute nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35j90dm66h3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1kxayvy</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Blue💙</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6zynv8q5h3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1kxa2ml</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>My gel nails keep popping off.</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypi8jl02vg3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1kx9ylm</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>My current set I did for me</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx9ylm</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1kx9vny</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Press-Ons🖤</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a86e6zgssg3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1kx932t</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>First attempt ever at doing French tips</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g204wn2xjg3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1kx721y</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Press ons and Nail Damage (HELP)</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx721y/press_ons_and_nail_damage_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1kx8msz</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Ring of fire?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9n4fawlafg3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1kx8fgc</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Kirby inhale!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usblkla6dg3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1kx7xlw</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Inspo vs what i made</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl69u2t48g3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1kx7sxy</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Goth os Coquette?:)</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx7sxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1kx7efj</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Some Press ons I made</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx7efj</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1kx6ytl</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Made bird of paradise press ons</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3hgumbqyf3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1kx6rzy</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>I needed a clean conference look ❤️</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx6rzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1kx6meb</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>my latest set🌃</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx6meb</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1kx6b9r</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Before and after</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx6b9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1kx5a8v</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Severance Nails 🐐👔📎</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx5a8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1kx5tqs</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Cat eye but French !</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx5tqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1kx5x5z</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>My new gel x extension set by @Zenrennails inspired by @amys.clients on instagram</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx5x5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1kx5un0</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Strawberry milk</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s05r9ozjof3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1kx59jj</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>First time having my nails done in a while</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b8b2yxd5jf3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1kx4x3f</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Is gel allergy inevitable?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx4x3f/is_gel_allergy_inevitable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1kx4xq4</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>I spent $15 on a home nail kit from Target - beautiful and cheap but so prone to lost nails after just a few days!!</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brxjb2nhgf3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1kx4p57</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>New mani what do y'all think?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85woi14cef3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1kx4o76</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>French Tip</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx4o76/french_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1kx4jmv</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>It’s been raining for DAYS but I’m feelin sun-shiny 🌸</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9f6nf4zcf3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1kx44ym</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Should I be concerned at how my nails look right now?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx44ym</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1kx48sx</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Wedding nails help</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx48sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1kx3z20</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Hello Lisa Frank</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx3z20</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1kx3aaw</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>y2k pink💕</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx3aaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1kx34v4</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Nails and cuticles</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx34v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1kx2yth</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>tried out pearl pat pat gel!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx2yth</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1kx2x5z</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>I peaked - Color Changing Velvet Gradient</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ereu3a7tye3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1kx2wrc</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Press on nails for long nail beds?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx2wrc/press_on_nails_for_long_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1kx2ukr</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Birthday nails🌙💕✨</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95wjxti8ye3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1kx2trc</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Beginner who needs help</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx2trc/beginner_who_needs_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1kx2rgh</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>What are some dark nail colors that work for summer time?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx2rgh/what_are_some_dark_nail_colors_that_work_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1kx21zq</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>I found a new addiction with press on nails 😅</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx21zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1kx1z2d</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Love these chrome</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6201quyqe3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1kx1hvx</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>whimsical goth inspired nails :)</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ilkchtyme3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1kx1n21</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Jellybeans</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heu3ov37oe3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1kx15ar</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Realized I matched the tractor color when I got home.</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx15ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1kx13tq</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wlfhul6yje3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1kx10f9</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Pedicure</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx10f9/pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1kx0jpq</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Why does this happen to only one nail on each hand?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5aawbmtjfe3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1kx0vj6</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>wanting to do my own nails with gel …</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx0vj6/wanting_to_do_my_own_nails_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1kx0l9i</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Help! Need advice for my wedding nails!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx0l9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1kx0pba</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Fresh gel set, in pink</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkx0zjtrge3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1kx0go1</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Strengthening under dip powder manicure</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kx0go1/strengthening_under_dip_powder_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1kx0c2s</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Please be kind</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ci1dllyde3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1kwza8n</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Home Manicure</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lh0vpinb6e3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1kwz5io</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Loving my new beachy set!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwz5io</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1kwxoc8</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwxoc8/new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1kwytq7</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Second time giving myself a gel manicure</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwytq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1kwykm7</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Nail day :)</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yb0e8zb1e3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1kwy68p</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>🍊 🐟</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwy68p</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1kwy5de</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Cateye again 🥳</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jmpq5bbyd3f1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1kwxhka</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Got inspired by latte art, this is my first attempt with blooming gel</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwxhka</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1kwxkbh</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Color Matched to Grandma's Sweater</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwxkbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1kwxhdn</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Why does Pinterest love showing me things I can't have? Looking for a similar color as this product in gel form (or any form that needs UV curing and longevity.) Any recommendations?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwxhdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1kwwczx</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Need advice</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwwczx/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1kwwylj</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>My Coke Zero inspired nails!</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwwylj</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1kwx11g</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>New set! 💙</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29ce0xzhqd3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1kwwgnn</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Is there an age limit on glitter?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/roul9fxgmd3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1kwwfmv</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Favorite sets of this week! Which is yours?!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwwfmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1kwwdrk</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Floral nails💐</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwwdrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1kwwcws</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>When life gives you lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwwcws</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1kwwaiy</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>pink alstroemerias</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usteeltbld3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1kww46i</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Star Crossed Lovers</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kww46i</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1kwvcij</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Gel nail lamp kit - recommendations</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwvcij/gel_nail_lamp_kit_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1kwvcet</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>A set I made for a friend</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21o9837ted3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1kwunki</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>love an ombré moment!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gojlsb0ad3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1kwuigb</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>🧜‍♀️🐚</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y96awwe09d3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1kwudg8</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>How to Stop Natural Nails Curling?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwudg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1kwtxgt</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Does the color look bad?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8sg6d36z4d3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1kwtiqc</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>How to remove glued nails without damaging the fake or natural nails?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwtiqc/how_to_remove_glued_nails_without_damaging_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1kwtb83</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Which shape is best?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwtb83</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1kwkgkf</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>How do you keep your natural nails strong?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwkgkf/how_do_you_keep_your_natural_nails_strong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1kwqppe</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Can I put on an extension?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwqppe</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1kwslrw</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Is there an update on the young lady that got maimed?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwslrw/is_there_an_update_on_the_young_lady_that_got/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1kwsegi</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>what do you guys think? i think she’s a amazing</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb5197iiuc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1kwrz3d</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Strawberry Shortcake 🍓🍰✨</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jt7aix0jrc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1kwrssn</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Made this super cute fruit set 💕</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwrssn</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1kwrrt8</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Newbie Press On Nail Sizing</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwrrt8/newbie_press_on_nail_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1kwrgp4</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Made Strawberry shortcake Nails Myself 🍰</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwrgp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1kwr9ef</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Not very original, but still super cute!</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwr9ef</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1kwr2r0</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Ink in motion 🖤</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkdgl14alc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1kwqxpj</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Colors</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwqxpj/colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1kwqabx</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>blueberry nails!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zs96zgxtfc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1kwn47v</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Help😭 what is it</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brpdlslfsb3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1kwjs4u</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Is this okay ?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hzh9zenwa3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1kwpchx</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>What do I ask for??</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez6424e79c3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1kwp54f</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>my nails have grown out alot but I don't know when I'll next be able to get to my nails place, what do I do?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fa0fbcmq7c3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1kwp19c</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Dip powder ruined my nails - what next?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwp19c/dip_powder_ruined_my_nails_what_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1kwpndo</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Best Gel Polish</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kwpndo/best_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1kwmhzu</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>different styles, which one do you prefer? 🫠👏🏻</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3ipai3dnb3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1kwlztn</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Can someone explain to me why this happens sometimes with chrome?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfiq5ohzib3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1kwlym4</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Can These Be Toned Down?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwlym4</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1kxb7e9</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Cyborg “dupe” comparisons</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxb7e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1kxb3ry</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Any recommendations for first ILNP order?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ge2touhc7h3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1kxb2cv</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer Nosferatu</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxb2cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1kxaiso</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>I’m still bad at “nail art”, but gotta catch em all</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3t2wtvmd0h3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1kxadws</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>May Mooncat manis</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxadws</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1kx762l</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Need help finding toppers</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx762l/need_help_finding_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1kx9pkc</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Do I have to stop doing gel manicures?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7t48ltqtqg3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1kx4cjr</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Ether dragon ~siblings~…?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jxutuj8bf3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1kx8j21</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Questions on magnetizing</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww4lo1f7eg3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1kx8iaz</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Please help me choose my 1st ILNP order! What will look good on me?!</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx8iaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1kx8be8</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Question about nail care</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx8be8/question_about_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1kx89kw</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>CARDBOARD QUEEN IS LEVIT THE QUEEN</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3fvfv2sdbg3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1kx886i</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Fauve Cosmetics - Muse</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mhs5k6p1bg3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1kx7bg7</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>{PR} -50 | Sassy Sauce shop release</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx7bg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1kx797r</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Yellowstone National Park Mani Ideas</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx797r/yellowstone_national_park_mani_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1kx78pl</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Copper patina or limited success woodscape?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx78pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1kx780h</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Polish for nail picker</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx780h/polish_for_nail_picker/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1kx72kp</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Cricut for nail designs</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx72kp/cricut_for_nail_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1kx6ppd</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Help finding a shimmer like this state-side?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dw79xfmcwf3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1kx61lz</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Delicate by Polished for Days</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx61lz</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1kx5m8n</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Does anyone have a good dupe for KBShimmer living my Zest Life?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he2m80rgmf3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1kx4tnw</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Emily de Molly sold out 😭</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx4tnw/emily_de_molly_sold_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1kx4iut</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Best primer/bonder/whatever it is for gel polish?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx4iut/best_primerbonderwhatever_it_is_for_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1kx497l</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space - can’t stop staring at my nails!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7pio9i4eaf3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1kx3zfa</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Nails on Nails lol (Sinful Colors - Queen of Beauty)</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3gtuum18f3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1kx3wic</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Some small wins today regarding polish mistakes.</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx3wic/some_small_wins_today_regarding_polish_mistakes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1kx3u2v</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>I Think They Wound Up Cute</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx3u2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1kx3pgz</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>This is too freaking pretty not to share...</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1g136dm5f3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1kx31t7</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>nail salon ruined my nails</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kx31t7/nail_salon_ruined_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1kwwj4r</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Do I still need a dust collector?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwwj4r/do_i_still_need_a_dust_collector/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1kwwc11</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Love for Voyage Hues</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rv23741kd3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1kx2tiy</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Gel help! I can't get my soak offs to soak off...</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx2tiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1kx2pxd</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Glass Stars</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmntrdg3xe3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1kx2m0s</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>nixie ✨</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx2m0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1kx2ap4</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Help me narrow down my cart??</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx2ap4</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1kx20bo</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Got bored of silver in a day…on to hot pink!🤩💗</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx20bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1kx1jfp</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>The Observer’s Paradox</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx1jfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1kx1gpu</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Rebuilding my collection after developing a gel allergy, trying out a darker spring look...</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xwvph4tme3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1kx18m1</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Strawberry milk nails😍😍😍</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ygkc9lkzke3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1kx0zqo</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>💫Epic Universe Mani☀️</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx0zqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1kx0n3x</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Does anyone have a dupe for Ethel by Cirque Colors? I'm devastated its discontinued</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87b2qplage3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1kx0kro</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Scattered flower design</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx0kro</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1kx0hva</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>ILNP - Deep Space 🩵💜✨</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s3lu00f5fe3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1kx0e3g</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Help—am I causing this?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8s40654dee3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1kwzgqi</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Love these Mooncat shades together 💙🤍</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwzgqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1kwzarp</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>DVN Graphite Grit / Dust to Dust</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwzarp</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1kwza5p</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>🩷🩷NEW ILNP COLLECTION!!!🩷🩷</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwza5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1kwz1ia</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Why do my middle fingers always break? This never happened before the previous salon ruined my nails.</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwz1ia</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1kwyddo</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>2nd Chrome attempt</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ic7v1i8xzd3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1kwy9up</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>The polish I wish I'd known about for my friend's "Maui sunset"-themed wedding 🌅</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9luv4wu7zd3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1kwy5f1</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Random mani #2: Overwhelmed by sparkles! ✨</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwy5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1kwx6e2</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>My Polish Regrets</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwx6e2/my_polish_regrets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1kwwzwy</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>A request for any maker’s lurking out there</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwwzwy/a_request_for_any_makers_lurking_out_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1kwwj3i</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Lurid lacquer order came in two days early and had a bonus polish that I didn't even order!</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwwj3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1kwwgls</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Space Oddity</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1c1hh9gmd3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1kww7aw</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Messing around before picking a new polish. Which “topper” is your fave?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kww7aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1kwvjna</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Artificial nail length while using regular polish?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwvjna/artificial_nail_length_while_using_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1kwv72q</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Love this color! ILNP Sunkissed</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwv72q</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1kwu6zu</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>I didn’t expect Fields of Lavender to become a new favorite</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hmtnglhr6d3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1kwto7t</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>A nail polish like this spoon?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwto7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1kwtjee</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>HOW DO I STOP TOUCHING THEM</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwtjee/how_do_i_stop_touching_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1kwtihg</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>I thought i was so smart buying a red jelly for a true red magnetic</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ulws7xq02d3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1kwsnjn</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>🍉🍉Watermelons🍉🍉</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwsnjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1kwsipg</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>The last of my limited edition FUN lacquer color.</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq1rpybdvc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1kwsfji</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>How was this done?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jvav3ruee53f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1kws5lx</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Is there a polish range that looks like sea glass?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hh27cdhtsc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1kwrj3z</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I'm in trouble deep</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwrj3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1kwqcw2</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Gold chrome powder - no gel, no lamp! Experimenting is so fun!</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwqcw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1kwq18k</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>“Cuticle” or nail protector tape tips?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwq18k</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1kwpxsy</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>I love Phantom Call but it pisses me off so much!</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwpxsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1kwptka</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>On the hunt for summer blues. This one's my fav so far</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2o6nouzhcc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1kwp4e6</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Blue ba da bee ba da dot</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ryia5zjk7c3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1kwox9e</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Clear nail polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwox9e/clear_nail_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1kwohx7</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Pistachio buttah</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwohx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1kwo7np</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Trouble with Cirque Jellies drying slowly</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwo7np/trouble_with_cirque_jellies_drying_slowly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1kwnu8p</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>worth the hype polishes?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwnu8p/worth_the_hype_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1kwnnte</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Magnetic magic</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x3bxvzhpwb3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1kwn7ta</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>ISO Holo Glitter Topcoat</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwn7ta/iso_holo_glitter_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1kwmao4</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>ISO the perfect neon green</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwmao4/iso_the_perfect_neon_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1kwlv26</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Absolutely changes my manicures!</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwlv26</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1kwlljj</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Please share your tips to make (regular) nail polish last longer</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwlljj/please_share_your_tips_to_make_regular_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1kwl0sk</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>my nail polish storage so far!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwl0sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1kwixm2</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Memorial Day nails: Painted Polish - Oh My Stars</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwixm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1kwix75</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Wedding nails, help and inspo</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwix75/wedding_nails_help_and_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1kwb8i4</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Looking for Hard Candy Dupes</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kwb8i4/looking_for_hard_candy_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1kwi928</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Utterly in love with this colour combination!</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0nz19if1ea3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1kxbl8d</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Labubu charm kawaii junk nails 🍭🎀🌈</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39gb10o7dh3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1kxb5xv</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>my latest press on set 🤍</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2lvhvg38h3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1kx9xs4</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Strawberry Milk set I designed for the strawberry season 🍓🥛</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0itpdw2htg3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1kx5j98</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Love my new set</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsqlzkuqlf3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1kx2wy6</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>I really love foil nails 😍</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6re0kfrye3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1kx1xy3</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Should I go back to the salon for a touchup?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx1xy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1kx1fzs</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Getting my nails done tomorrow, drop some inspo pics!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kx1fzs/getting_my_nails_done_tomorrow_drop_some_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1kx0ry9</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>A few sets I’ve done at school lately! ✨💅🏽</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kx0ry9</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1kx0oxp</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>hand painted by me!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zc8artoge3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1kwzw7h</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Help! What is a likely price for nails like this?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rilrajlae3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1kwzmaq</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>What type of polish is used in these kinds of nails?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avf2559q8e3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1kwxock</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>I loveeeeee nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to0xx38zud3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1kwwhye</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>When life gives you lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwwhye</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1kwvegc</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>What do people think?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgshd6c7fd3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1kwvbl0</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>These Are the Top 10 Nail Trends Dominating Pinterest in 2025</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kwvbl0/these_are_the_top_10_nail_trends_dominating/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1kwsndc</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Latest commission for fishing lure nails 🤩👩‍❤️‍💋‍👩</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18ha8ym7wc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1kws3ux</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>My set for a music fest</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kws3ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1kwr43f</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>🫐🐞🍃</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjr2gi0jlc3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1kwqhj6</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>psych nature nail set!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kwqhj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1kwpay4</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Hi, so I painted my nails into the Squid Game X-O votes and wanted to share it ❎🅾️</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hfppbfw8c3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1kwltgc</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Vacation nail ideas pleaseee</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kwltgc/vacation_nail_ideas_pleaseee/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1kwjpp6</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Here’s some more beginners work 🤦🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bjfwtrwva3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May 29 08:12:40 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_01.xlsx
+++ b/data/collected_data/2025_06_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C716"/>
+  <dimension ref="A1:C909"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12605,6 +12605,3287 @@
         </is>
       </c>
     </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1ky4v41</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>The best nail I did so far</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywudcyyhdo3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1ky4on0</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Sanrio</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns6ci9scbo3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1ky4l3d</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Was this my fault</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ky4l3d/was_this_my_fault/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1ky4hvq</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Which shape looks better?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky4hvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1ky43h5</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>which nails look better on me? 😅</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky43h5</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1ky3np1</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>My recent set!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/angdwb74zn3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1ky3gmm</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2j605utwn3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1ky3da5</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>recommendations on where  to buy from plsss ( indian company mostly pls 🙏)</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ky3da5/recommendations_on_where_to_buy_from_plsss_indian/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1ky31xc</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>This is the manicure I got today I think it looks good</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suysn8wxrn3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1ky2vd6</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>My most recent</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky2vd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1ky2eka</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Criticize these nails in one sentence.</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oxq85yotkn3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1ky2rj4</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Rainbow nails! 🌈 mix of gel and regular polish (left to dry for adequate time)</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky2rj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1ky2deo</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Just got new nailssss</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky2deo</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1ky1ype</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>First time builder gel and natural nail</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky1ype</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1ky1mjn</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>i made Fallout inspired nails!!!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky1mjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1ky1mx0</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>What do I ask for?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuq5i61qcn3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1ky1pbb</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer - Marigold 🦉</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky1pbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1ky1ix6</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zog6xllbn3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1ky1i1o</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Can I still get my nails done if I have a cut in it?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ky1i1o/can_i_still_get_my_nails_done_if_i_have_a_cut_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1ky1eu1</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Just finished this design hope stays enjoy this</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l10gg6qian3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1ky14zw</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>This was my fav “fancy” neutral mani so far</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3mbglru7n3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1ky0mjm</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Lavender lemonade 💜💛</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky0mjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1ky01j3</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>just got my nails done and now im obsessed</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v751a0chxm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1ky01hv</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Got my nails done and a week later at tea with the girls, I realized my bestie had the same mani. Such a fun little surprise!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky01hv</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1kxzksp</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxzksp</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1kxz0cr</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Builder Gel on Press Ons?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxz0cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1kxz4yw</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Nails for Beyoncé</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5ja9uk9pm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1kxylvn</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>First attempt at doing my own press-ons!</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vb5d5ukkm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1kxybc2</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>First set w/a new tech 💖💅</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0wkuzmuhm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1kxy19f</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Nail Tech freehanded this</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9do958kfm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1kxy0sk</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>French tip first timer!</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxy0sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1kxxzez</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Kawaii junk nails I made</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06qq7nu3fm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1kxxsme</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Milky White?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zqd3h9hdm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1kxx07l</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>painting inspired nails!!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxx07l</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1kxx4ue</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>They like it ?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6idw6lr7m3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1kxwjkw</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Question?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxwjkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1kxwk68</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47mpopvz2m3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1kxwidj</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>DIY natural nails</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxwidj/diy_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1kxw7eb</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>My two favorite sets done by my tech!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxw7eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1kxv3ht</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Eveline 3 in 1 Nail Whitener</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxv3ht</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1kxvyla</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>How long should I wait to apply fake nails?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxvyla</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1kxvsog</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Gel manicure ✨</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ov0azojpwl3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1kxvgut</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>What’s this mark</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2qafvw2ul3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1kxv4vi</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>First time doing marble effect</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytfeakphrl3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1kxue79</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Should I get gel press ons on my nails?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxue79/should_i_get_gel_press_ons_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1kxtwpr</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Au naturel 💙</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxtwpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1kxtucl</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Love my nail set</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kgsnfughl3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1kxtp4f</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>I got a gel manicure two days ago and I’m disappointed with how grown out they look</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha16b7zcgl3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1kxtlko</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Nails to go with this dress? For prom!!</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxtlko</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1kxt2ac</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>paid with my left kidney but i think it was worth it 💅🏽</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqhmrijqbl3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1kxsvot</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>My tech popped off with my birthday nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzxcffvdal3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1kxsn87</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Atlantis Themed Set</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxsn87</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1kxsa6m</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Swirly pearl French tips and their inspo</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxsa6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1kxs9o4</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Set done for clients SZA concert!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6fj2sw26l3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1kxs15h</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>😍</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxs15h</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1kxry30</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My current nail set (better pictures)</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxry30</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1kxrd47</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>In dedication to the People's Republic of South Yemen 1967-1990</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxrd47</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1kxreud</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Is this shape flattering on me? If not what shape do you think would look better?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv0xslz20l3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1kxr2sn</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Some matte opals this week</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn9nu49pxk3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1kxqvsv</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Green cat eye</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6wyxdh5dwk3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1kxqncm</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Seashell Nails!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxqncm</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1kxqb1m</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Chrome nails yes or nah ?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfp7j00ask3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1kxq2c9</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Working man’s nails lmao</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxq2c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1kxpwrw</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Fresh Spring</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxpwrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1kxpwrt</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Attempt after a long time</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxpwrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1kxpk92</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>pansexual pride nails 🩷💛💙</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxpk92</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1kxpeja</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>I’m totally in love with this set 🫠 btw they r my natural nails</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m04dq8nvlk3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1kxou09</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>How should I fix my nails separating from acrylic?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxou09</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1kxoscz</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Are my nails not cat eye enough?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zx79bojhhk3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1kxon97</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>what I got vs inspo (found on Pinterest @kash)</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxon97</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1kxludt</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Dip question</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfxdf3wswj3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1kxmfnh</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Will my nail bed become regain its natural lightness?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie4cyw0x0k3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1kxoe7o</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>I need help!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxoe7o/i_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1kxmh2n</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>6 Weeks, 10 Fingers, and a Lot of Hope: My Nail Rescue Journey</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxmh2n/6_weeks_10_fingers_and_a_lot_of_hope_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1kxo6cc</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Engagement Nails</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxo6cc/engagement_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1kxo0vs</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>First time doing 3d details🙏🏻🌸</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vdgekmv3ck3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1kxnyuf</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Cateye over chrome</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ujc2f74pbk3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1kxnxgg</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Lavender Butterfly Dreams</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxnxgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1kxlzvp</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>best low-tox nail products used by professionals</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxlzvp/best_lowtox_nail_products_used_by_professionals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1kxnjr2</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>i need help with no this acrylic nail!!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekg1a0xs8k3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1kxn7t6</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Current Nail set :)</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxn7t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1kxn469</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>First time doing press-on nails 💅 (the colour IRL is actually a mauve/muted berry tone, not brown)</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxn469</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1kxn3s5</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>I started making press ons in December and have been thinking about doing this since then</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqpav7mq5k3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1kxmvqj</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Obsessed 🥰</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y3cdqp34k3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1kxm6q7</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxm6q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1kxm60x</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Thin acrylic on top of natural nails?</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxm60x/thin_acrylic_on_top_of_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1kxlccu</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>What are your favorite press ons brands with lamp curable nail glue??</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxlccu/what_are_your_favorite_press_ons_brands_with_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1kxk12b</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Presson nails set inspired by my pet rabbit 🐇</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxk12b</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1kxk110</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>How can I be more assertive about my nails?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxk110/how_can_i_be_more_assertive_about_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1kxkkvd</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Acrylic nails infills</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxkkvd/acrylic_nails_infills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1kxka2s</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Tiny little nails</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42mnrwzslj3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1kxk1nq</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>🤡🤡🤡</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk24ebx3kj3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1kxbo43</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Nail care between sets</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/waps2ei8eh3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1kxh40s</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Help with nail shape</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxh40s</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1kxibrj</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Flat Nails</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ii60gq1u7j3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1kxi2or</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Feeling berry cute today!</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxi2or</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1kxe0kq</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Vettsy</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxe0kq/vettsy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1kxjbjr</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>New press on</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obb0ge51fj3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1kxj7wh</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>At home nail set after feedback here!! Kinda giving bridal nails in 2015 but i'm not mad about it</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxj7wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1kxj3x5</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Why do people use press on nails?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kxj3x5/why_do_people_use_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1ky38v5</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>trying press ons while growing out ✨</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4he13j5cun3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1kxrqnc</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>My nail polish looks bubbly</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m197hove2l3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1kxy6gf</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Essie Rubies (Ruby?) Slippers Bottle Misspelling</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxy6gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1kxz515</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>My first successful stamp ❤️</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3lwzd7apm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1ky23cd</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Can this be done with regular polish?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ai4qfqhghn3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1ky1w0h</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Mooncat Donations</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ky1w0h/mooncat_donations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1ky1oie</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer - Marigold 🦉</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky1oie</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1ky1jc6</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Wind Waker Mani</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky1jc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1ky1glf</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>These are my own nails, painted by myself, so I’m probably out of my depth, but I’d like advice.</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gn8rxgzan3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1ky17uu</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>From my first Lyn B Designs order! I'm so impressed! And I couldn't resist adding a topper</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky17uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1ky0sql</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>You know who it is</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky0sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1kxzpqo</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Leave that $@#% to the professionals</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y3me1cj2dk3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1kxze9n</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>OPI or Essie?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxze9n/opi_or_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1kxzbbc</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Seche Vite turns yellow?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxzbbc/seche_vite_turns_yellow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1kxz3ht</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>a field of wildflowers</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ycd6hbfmm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1kxyycv</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>You can only choose one, spend $100 at ILNP or save it for July PPU?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxyycv/you_can_only_choose_one_spend_100_at_ilnp_or_save/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1kxy5y2</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Burdock &amp; Buckthorn in the sun 🌿🫐🌱</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxy5y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1kxy50w</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Took a break from nail art!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxy50w</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1kxy2gp</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>ISO topper made of primarily silver hexagons</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxy2gp/iso_topper_made_of_primarily_silver_hexagons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1kxwwhc</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Translation needed</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxwwhc/translation_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1kxwtjy</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>OPI Nail Envy: if It’s clear is it bad? And do you like the product?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxwtjy/opi_nail_envy_if_its_clear_is_it_bad_and_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1kxwoor</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>What I wore in May!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxwoor</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1kxvirb</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Eveline 3 in 1 Nail whitener</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxvirb</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1kxvgbp</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Had fun with two thermals today</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxvfn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1kxv6is</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Large growth points</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxv6is</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1kxv4wo</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Ooooh - inexpensive polishes coming through!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxv4wo</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1kxuzj6</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Dad's Patio, 2019 (May random GWP / June release)</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxuzj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1kxuygk</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Lemon Brain</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxuygk</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1kxuvik</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>painting inspired nails!!</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxuvik</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1kxueuk</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>LynB Heuristic is so underrated</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c9rkspqrll3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1kxu1a3</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Mooncat - Quicksand’s Embrace</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uz84ev6vil3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1kxtuao</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>PFD - So Close 🩷</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxtuao</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1kxtbbi</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>✨🟣 Crystal Bold Rush 🟣✨</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxtbbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1kxt8yg</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>ILNP is slaying Mooncat right now</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxt8yg/ilnp_is_slaying_mooncat_right_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1kxspru</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Star Destroyer! 🤩</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxspru</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1kxs47c</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Nails curving and lifting</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnymu9405l3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1kxrtug</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>PP/Atomic Polish - Victoria Amazonica</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxrtug</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1kxrf6q</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Rainy day shorties ☁️</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxrf6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1kxqq4x</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Help identifying this OPI mini</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulb1vtm7vk3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1kxq6f3</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>The perfect manicure for the last coupl of weeks of spring</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxq6f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1kxpz8g</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>I expected to be disappointed but…</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k71a3m4ypk3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1kxpwkp</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>My whole collection!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud9al6xepk3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1kxpa83</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Weird pinkie thing I’ve only noticed since taking mani pictures …</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxpa83</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1kxp7x1</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Halsey concert nails</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxp7x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1kxol7x</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>F*ck This Sh*t👹</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxol7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1kxo5e6</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Deeply disappointed in secondhand Ultrahot. Suggest me a dupe?</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxo5e6</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1kxo32g</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Help. My nails are awful.</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpru745jck3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1kxnx8p</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>this mani tried my patience</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxnx8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1kxnsbi</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Tiny Emo Mani</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxnl6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1kxnnpx</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>My husband says they look like cows…I mean, he’s not wrong 🐄</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4q7m4fk9k3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1kxnnfc</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Lei One On Me 😍</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxnnfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1kxn6ck</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>I recreated Cirque Colors’ post: aura nails but make it neon (Vice 2025)</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxn6ck</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1kxmwz8</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Fishy friends</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxmwz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1kxml5d</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Thank you to the person in this subreddit who recommended Bramble and Burr to me!!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxml5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1kxma3i</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>I Got You Babe</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxma3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1kxm95c</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Off the Deep End</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxm95c</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1kxm1t5</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Thrift finds!🛒💅🏾</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxm1t5</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1kxluqo</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Springy Summery Nail Stamping</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxluqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1kxlrig</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Help me get rid of ILNP</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxlrig</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1kxlqoj</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Can you use non-gel polishes like the ILNP magnetic to create the cat-eye look? I only see line shapes with ILNP, not the cat-eye effect.</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxlqoj/can_you_use_nongel_polishes_like_the_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1kxlgod</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Flakies on flakies</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxlgod</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1kxjmhy</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Close enough?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxjmhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1kxjg59</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>💚🦓Lydia B. Kollins🦓🩷</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxjg59</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1kxj5p3</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>A little bit of sparkles and thermals</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxj5p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1kximy3</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>What do you call this finish? Any similar polishes?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kximy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1kxil0f</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Should I worry about rusting if I add "normal" stainless steel balls to polishes?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxil0f/should_i_worry_about_rusting_if_i_add_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1kxify1</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Jump scare from sassy sauce</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxify1/jump_scare_from_sassy_sauce/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1kxi4zi</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Drop your oil recommendations pls :) and any other tips for growing out nails!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxi4zi/drop_your_oil_recommendations_pls_and_any_other/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1kxhs91</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>The Brazilian manicurist way of painting nails</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxhs91/the_brazilian_manicurist_way_of_painting_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1kxhpc3</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Gel Gel Go Away so I can't paint another day. Help! Can't get my gel all the way off...</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxhpc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1kxg7fl</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Those who paint press-on nails, do you buy clear or white coloured nails?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kxg7fl/those_who_paint_presson_nails_do_you_buy_clear_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ky08t7</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>I run out of gloves so gotta occupy myself somehow</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky08t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ky06ye</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Britney Spears Press On Nails on Instagram @nailart.x.victoria</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5r2i27xym3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1kxzzcd</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>My first gel x tips</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ggqgflwwm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1kxz1ny</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Pride inspo</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kxz1ny/pride_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1kxyw3h</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Stitch! 💙🩵</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epbmx0l3nm3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1kxxhnw</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>finally cut my brush bristles and the lines are crisppp</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdquge6tam3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1kxxexh</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>This was from Halloween ,they like it ?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61eq1qy4am3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1kxxbap</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Barbie Goth Chic</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxxbap</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1kxx9zi</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Ok here’s another one 🫣😝</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t9vucdky8m3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1kxwuei</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Easter Nails</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh4jjfka5m3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1kxwko4</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Scorpion babies 💅🏼 🦂</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxwko4</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1kxtx71</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Minecraft dip</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwr20nizhl3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1kxsvst</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>How do we feel about these?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsonkdkfal3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1kxsotj</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Atlantis Themed Set</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxsotj</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1kxq0q9</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Help getting pictures of shifty designs?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9y0cplu8qk3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1kxpt7g</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Fresh spring</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxpt7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1kxpa92</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Natural shiny ❤️🫶</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwchv4m0lk3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1kxoz3j</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Should I make these glossy?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4yoj7vtik3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1kxnz9q</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Strawberries and Cream 🍓</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipzy9m8sbk3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1kxnw75</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>I’ve been doing my own nails for a few years now, but only recently got into the designs after switching jobs!</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxnw75</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1kxlea1</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>What is this nail shape?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zap0xlfmtj3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1kxkk4s</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>hello kitty y2k nails</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kxkk4s</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May 30 08:12:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_01.xlsx
+++ b/data/collected_data/2025_06_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C909"/>
+  <dimension ref="A1:C1114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15886,6 +15886,3491 @@
         </is>
       </c>
     </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1kyyq9j</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Happy with how they turned out</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjpai805nv3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1kyyga0</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Any tips for broken nail besides tea bag method? :(</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyyga0</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1kyxzfa</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Why I can’t find a nail salon who does a good mani on natural nails</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kyxzfa/why_i_cant_find_a_nail_salon_who_does_a_good_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1kyxvcw</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>June set is ready</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbskw6nhcv3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1kyxihe</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Which nails should I do for my anniversary next week?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyxihe</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1kyx6pj</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Can’t tell if I like the colour or not! Help!</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rch06ge4v3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1kywn06</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Looking For Acrylic Nail Brand Suggestions</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kywn06/looking_for_acrylic_nail_brand_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1kyvlir</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>How do I get these off??</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kyvlir/how_do_i_get_these_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1kyu2p4</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>I have come to the conclusion that nail glue is a scam and doesn’t work for any one.</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kyu2p4/i_have_come_to_the_conclusion_that_nail_glue_is_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1kyvk31</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>abstract nails</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5zkdh63mu3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1kyvjf6</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kyvjf6/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1kyunwu</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>What do we think? 🌊</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nbki4h0du3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1kyukmm</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Making my own press on nails</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbqmivz4cu3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1kyuckb</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>My Natural Nails (10 month journey)</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyuckb</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1kyu5yh</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>How much would you charge?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyu5yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1kytqoo</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Cow print meets Loki</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d3loz364u3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1kytd24</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Good GEL nail sets?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kytd24/good_gel_nail_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1kyt3m5</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Do we like them?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyt3m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1kysy15</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Is this normal for a Russian pedicure?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kysy15</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1kysuae</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>New nail lady should I go back?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hpua9d3ovt3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1kystn3</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Engagement nails! 🥰🌹</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kystn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1kysqus</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Got cat eye for the first time</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kysqus</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1kyqcp6</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>how do i make the “caps box” lid attachable? is it even possible?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/txd8pshz9t3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1kysjun</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Removing UV polish from Biogel nails?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzabbouftt3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1kyrs97</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Summer Nail Inspo?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wf8nyh4nmt3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1kys1nz</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>First gel set in awhile</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kys1nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1kyrj2v</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>I love nail day 💙</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkus1ilckt3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1kyrio3</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>I did my own nails again….</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkye0k69kt3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1kyrfk5</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>I love my simple whimsy nails</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsw10dmgjt3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1kyrcim</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Summer nails!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48cgf5tqit3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1kyr8vs</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Going to get my toes done for the first time, cut them too recently. Need help!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kyr8vs/going_to_get_my_toes_done_for_the_first_time_cut/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1kyr6q2</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Back to my neutrals, after trying red, and I’m loving this set</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/474c251aht3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1kyqz9q</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Picture of my nails when I was swimming today</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prsy7hlfft3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1kyqnrw</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Help! What Emily de Molly blue is this?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n30jfpilct3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1kyqjmd</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Beachy summer vacation nails</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyqjmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1kyqj8g</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Arcana My Life As A Shrimp - mesmerized, enchanted, beguiled, obsessed 🌈</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o2o0uxqhbt3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1kypzf5</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Mario stars! 🩷🌟</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kypzf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1kyptgp</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Being taken advantage of?? Help.</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyptgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1kypecs</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Happy birthday to me! 🥰</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kypecs</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1kypeak</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Freestyle! Prompt was make em blue!</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kypeak</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1kyp4oz</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Nail polish color request!</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kyp4oz/nail_polish_color_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1kyp0qn</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Olive skin ppl: what are your favorite DND polish colors?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tdgystsys3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1kyoy7j</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Handmade Kuromi+ Cinnamoroll 🩶</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qw85ogv8ys3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1kyov5d</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>The shimmer</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tcr2bmsgxs3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1kyob7x</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Guess the price</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyob7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1kyo9zl</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>sheer pink manicure 🌸</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyo9zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1kyo58h</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>My first press ons!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0ox6jaors3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1kyo548</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>So i went i little out if my confort zone….. but i may say thata i love them</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1k3v6nmrs3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1kyo42i</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Pretty In Pink</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktfyr8ders3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1kynxix</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>birthday nails!</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtp2kvuzps3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1kynw0i</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Tried Press Ons! What do yall think?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd2ln2ynps3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1kynryp</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Orchid nails!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujotnz3ros3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1kyjny5</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Wedding nails - HELP!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5gcdkmrur3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1kymf4l</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Would gel nail polish solve acrylic nail splitting?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kymf4l/would_gel_nail_polish_solve_acrylic_nail_splitting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1kyl5lk</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Painted a Lilo &amp; Stitch set in honour of the live action 🥰 3d Surfboard anyone 👀😊</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjszqoih5s3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1kykw5o</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Why do my nails keep doing this?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z1jxcyk3s3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1kyg4xx</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>What shape should I get?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxcywtn06r3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1kyn9eo</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Nail ideas :p</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugvbzr6tks3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1kyn5xf</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>OBSESSED with this combo 🤩</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyn5xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1kylffo</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>I did a nail art set inspired by my favorite Panic! At The Disco album!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kylffo</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1kymfvw</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Update: I added a french tip and i think i fixed it</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1hxkikres3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1kymcn8</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Amy good?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrtkcsi3es3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1kylzyo</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Im obsessed</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kylzyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1kylx09</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Long time lurker, first time poster</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r09sfapwas3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1kyl06q</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>AI designed my mani</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3y1h9se4s3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1kyht3o</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>I had a nail travesty this morning</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt0gpizshr3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1kykr2l</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>What are these "bumps" in my nail shape</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kykr2l/what_are_these_bumps_in_my_nail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1kyf1bk</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Did some nail art for my favorite Panic! At The Disco album!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyf1bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1kykicn</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Today's color theme was orange 🍊</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kykicn</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1kykc5o</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>I'm obsessed with my dried flower nails 😍</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2d6jgrlzr3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1kyjya3</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>3rd attempt at doing my own acrylics</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20hcc3ptwr3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1kyjtyn</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Is this acceptable?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxqsuykyvr3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1kyjmnc</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Simple, but effective💅</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyjmnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1kyjld9</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Nail sticker question</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1i00fc79ur3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1kyj6ve</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>100% copied but still proud</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyj6ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1kyj1yg</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Loving this new set 😍💅</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw52gvciqr3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1kyix05</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Is This Normal? Builder Gel?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyix05</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1kyill6</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Round or almond?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyill6</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1kyikah</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Square or round?</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyikah</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1kyhw2p</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Feeling the butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o53kpg2dir3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1kyh2w2</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Protect my nails!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kyh2w2/protect_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1kyh0w6</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>I give up</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyh0w6</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1kygmvv</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Fairy nails have been popular lately🧚</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kygmvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1kyglkf</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Which shape fits me best ? Oval, almond or squoval</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyglkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1kyg38z</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>I did my sister's nails :3</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vzxdnu3o5r3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1kyg3te</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>New set for my upcoming Stray Kids concert ❤️</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyg3te</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1kyflh9</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iz3oq5ha2r3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1kyfgwl</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>French Mani As A Wedding Guest</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kyfgwl/french_mani_as_a_wedding_guest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1kyefj6</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Week old manicure</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtz7yko3uq3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1kyef51</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Almond or square?</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyef51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1kyeeg3</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Just painted my nails. Not a 100% clean job, but I love the colour.</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyeeg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1kye7x0</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Builder gel mani!</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kye7x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1kydz2k</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>What nails to ask for if I go once a year?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kydz2k/what_nails_to_ask_for_if_i_go_once_a_year/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1kyd947</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>The full bday set🎂💫</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyd947</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ky9iuq</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Still new to doing my own tips.. how do I stop them from separating/lifting at this point? And a couple other questions…</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68u6km4rsp3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1kycg66</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>are my nails too damaged?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mivswulvfq3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1kyc3d2</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Which shape is better?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8s1nu6jbdq3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1kybhf6</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kybhf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1kyb6r3</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>DND Mermaid Collection: Dark Aqua 💦✨</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyb6r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1kyb67p</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Stuck at home for weeks due to health, making my nails pretty made me feel a little better</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kovc6cc6q3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1kyxy7l</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Does anybody know what she uses on her nails under polish/have recs?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyxy7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1kyxwwv</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Got some nail stickers and I'm afraid to love them to much</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyxwwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1kyx2ns</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>EdM Check It (Thermal)</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyx2ns</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1kyx0gz</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>ILNPs rosewater + Mooncats not today satan on ring</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6o3kzjsv1v3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1kywqf8</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Jump start on pride month!! 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5krz1k4zu3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1kywpuw</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>ILNPs Pebble Path ✨</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k8eplg4ayu3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1kyvqzx</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Dupe Request for OPI’s Guy Meets Gal-veston</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.makeupalley.com/product/showreview.asp/ItemId=140388/Guy-Meets-Gal-veston/OPI/Polishes</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1kyvqry</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>New polish</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkskhxe2ou3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1kyvd8x</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Pain management mani 💚</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izz7sap0ku3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1kyv7p0</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Grandmanicure!</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyv7p0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1kyutm4</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Is this a real polish? Can anyone help me find it??</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2oda702neu3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1kyut2n</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Painted press ons for my friend!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyut2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1kyufdd</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Wished for Tomorrow</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucrpw82qau3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1kytyce</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Clionadh Niello!</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kytyce/clionadh_niello/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1kytnrk</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>I just realized the Essie brush is also twisted. 😤</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oahz4a6e3u3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1kytfd1</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>wasn’t expecting such crazy shifts from norpsilocin but wowwww</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kytfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1kyt1c5</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>shiny skittle w/ a touch of multi chrome</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyt1c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1kysq52</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Cosmic Polish is starting US shipping next week! 🤩</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2tf4108yut3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1kyscay</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Can we like...make anti- cleanup nails a trend?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc71l9clrt3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1kys2xo</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Birthday Mani ft. my Birthday Gift</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x8d0gnkapt3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1kys26w</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>✨️🧲ILNP Illusions[*PR*]🧲✨️</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kys26w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1kys1i2</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer “The Fields and Forests of My Youth” after 5 days of work</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kys1i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1kyrbdo</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Anniversary Mani</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyrbdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1kyr5ud</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Nailtiques wider replacement brush?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kyr5ud/nailtiques_wider_replacement_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1kyr09m</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Most similar polish to Deborah Lippmann's Space Unicorn?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kyr09m/most_similar_polish_to_deborah_lippmanns_space/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1kyqcrh</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Sassy Sauce must haves?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kyqcrh/sassy_sauce_must_haves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1kyq2hc</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>🪨 ZEN 🪨</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx1js1kn7t3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1kypzyt</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Has anyone tried these?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7ewhz927t3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1kypwqy</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>ISO polish that looks like this lobster omg</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kye8gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1kypdtt</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Unleashing my inner parrot with this neon green from 1422 Designs</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kypdtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1kyp8yw</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Collection, so far! Just posted all the individual swatches on r/piggypaint!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4aykd9nx9k3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1kyoomk</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Princess Blue</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyoomk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1kyoe0o</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Not sure what I was going for here</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyoe0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1kyo9so</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>My First Post</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbxxl0hvqs3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1kyo7xr</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>BKL Bog Dweller</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyo7xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1kyo3av</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Green skittle 💚</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyo3av</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1kynz3u</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Help me find the ultimate chunky glitter nail polish for my toes</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kynz3u/help_me_find_the_ultimate_chunky_glitter_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1kymyhl</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Arcana My Life As A Shrimp - mesmerized, enchanted, beguiled, obsessed 🌈</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l7gcl29eis3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1kympc5</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Eleanor Doesn’t Wanna Talk to You</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kympc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1kympam</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Are these ILNP Skate Date dupes?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kympam</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1kym9z2</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Top coat recommendations</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dnizfajds3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1kylx0y</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>My take on the viral "Ceramic Tile Nails" (with a bonus #mynailsandmytlc)</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kylx0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1kylun2</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Does BKL sell out super fast?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjs8uucgas3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1kyltuf</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>I’ve been enjoying playing with layering!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyltuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1kylnd0</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Unintentional matching with Maelstrom</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2einnbz8s3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1kyl7z8</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Lazy nail art: Swirl manis</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyl7z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1kykslo</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>The Minecraft Potions Jellies set by Plus Life Lacquer 🌈⛏️ releasing June 1st at 3pm PST.</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kykslo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1kyjy5i</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>My first Lurid 🤩🐅 On the Prowl</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyjy5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1kyjr4r</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>🛍️ Reveling in Mall-stalgia - ft. the Meet Me At The Mall collection from Prism Parade [PAID PR || AD]</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyjr4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1kyjok1</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Sagebrush🍃🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyjok1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1kyj99e</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Not sure if I love this combo, but oh well 🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyj99e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1kyii39</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Non Gel Nail Polish To Achieve Look In This Photo.</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2f9k03nmr3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1kyi9xh</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kyi9xh/is_this_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1kyi3dt</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>rainy days ✨</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyi3dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1kyi1o1</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>BKL’s Bog Dweller, like little glass gems on my fingers</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hbq4auofjr3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1kyhx5f</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Every time I wear a new polish I decide it might be one of my favorites</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9buws5ikir3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1kyhm0q</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Please add-to or remove from my ILNP purchase!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96srfia8gr3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1kyhlxd</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Glowy Cookout Wear</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/znwgqexegr3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1kyheas</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Timing on French nails</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kyheas/timing_on_french_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1kyhahr</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Love the trend of showing all your manis for the month--this made me realize how often I change my nail polish</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyhahr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1kyh5mo</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Holo Taco's Never Tide Down and Mooncat's The Sea Between Us comparisons?</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kyh5mo/holo_tacos_never_tide_down_and_mooncats_the_sea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1kygxth</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>that GLOW? hello?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kygxth</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1kygxed</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>PPU Rewind Spoilers</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kygxed/ppu_rewind_spoilers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1kyfv1t</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>illusions collection (gifted pr)</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyfv1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1kyfpuy</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>help me narrow down my cart</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyfph6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1kyfhlc</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>First time trying almond, any advice?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyfhlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1kyf3u7</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>please help with a good quick dry top coat</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kyf3u7/please_help_with_a_good_quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1kyezkg</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Whoops, my EdM cart got out of hand.</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyezkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1kyec67</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Anyone else use BEL London Laqueur ?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kyec67/anyone_else_use_bel_london_laqueur/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1kydup2</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>We have swatches!!! ILNP Illusions</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kydup2/we_have_swatches_ilnp_illusions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1kydti4</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Cupcake Polish Disco Dust</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zi8sh46mpq3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1kydn9t</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Looking for gel sheer-ish nude-pink recommendations!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kydn9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1kydk0j</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>All my May manis</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kydk0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1kycwut</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>I love this polish but its still so lumpy after 2 coats of topcoat..</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kycwut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1kyc1np</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>OH MY GOD 😮🥰🥰🌸</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyc1np</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1kybtrv</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>ILNP Clover 🍀</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kybtrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ky9zy8</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Can anyone identify this color</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eecyh0lvwp3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ky9o8h</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Best one coat white?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky9o8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1ky8kc9</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>European Indie / Small Brands?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ky8kc9/european_indie_small_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ky889b</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Dracula nails</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky889b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ky7pg3</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Could this yellow spot thru my pinky finger be nail fungus?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h25pqej1bp3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ky6gow</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>First time trying linear holo - it really tickles a sweet spot</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ky6gow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ky647x</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Be careful of fake dupe sites! (Starrily right now)</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ky647x/be_careful_of_fake_dupe_sites_starrily_right_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1kyyr9j</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Tips on making press ons</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyyr9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1kyy4nl</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Loved this trip — and purple’s my favorite! 💜</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyy4nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1kyvhrw</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>pink 💕</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7trsyfelu3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1kyv2r4</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Waiting for the month of October to make beautiful and spooky designs @isabellanails</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyv2r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1kyuyo7</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>🌸🍃🪽🌅🪴</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gbe752yfu3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1kyuax8</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Freestyle set</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbaxinki9u3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1kysk9q</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>In Memoriam: I did this nail between clients and messed it up basically the moment I touched my efile, so it lives on in this one photo.</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv4e8onjtt3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1kyqj3l</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Felt like painting nail tips 😊</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5haml5hbt3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1kyqisa</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Beachy summer time vacation nails</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyqisa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1kynjxo</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Finger nail trauma</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kynjxo/finger_nail_trauma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1kyn2xg</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Do you like the color blue on your nails?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1j9irzygjs3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1kymv6x</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>What do i tell my nail artist to do to get these nails?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yor8laguhs3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1kylqrb</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Painted a Lilo &amp; Stitch set in honour of the live action 🥰 3d Surfboard anyone 👀😊</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kylqrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1kykhbm</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>A new set I did on myself🤍</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnl16wdn0s3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1kyk3ax</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>junk nails</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i3g2a8txr3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1kyhfef</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>My girl did this set for $70 b4 tip 🥹❤️</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyhfef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1kygs0d</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Stained glass practice ✨</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hy4vlxjar3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1kyfkfb</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>This was the very first set I made ❤️🧡💛</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cjdx5j32r3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1kyd6dx</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Biab nails</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyd6dx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1kyccys</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>A few of my most recent client orders ❤️ I love love love making nails.</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kyccys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ky808s</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Celebrating Britney’s album Oops I Did it Again, as it turns 25 this week!</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4w9sve6ep3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ky5upm</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>How to achieve with gel and powder?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6x4o7wjpo3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May 31 08:11:12 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_01.xlsx
+++ b/data/collected_data/2025_06_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1114"/>
+  <dimension ref="A1:C1318"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19371,6 +19371,3474 @@
         </is>
       </c>
     </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1kzrt9r</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Can’t stop looking at them</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ge5dhp26r24f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1kzrckz</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Help a guy out</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzrckz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1kzqce5</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Can mold grow in clear water-based polish?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9v1p43dk924f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1kzqwfo</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Kitty stickers 🐱</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzqwfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1kzqwf5</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Today's set - dip and handpainted</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgxud533g24f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1kzqs6s</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzqs6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1kzpz5j</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>First time painting nails!!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzpz5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1kzpwah</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Help :(</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzpwah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1kzppn5</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Affordable Gel Polish for Press-Ons?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzppn5/affordable_gel_polish_for_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1kzpklt</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Love how my press ons looked today!</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvawqj6q024f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1kzp4zi</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>april nails + request!</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5lbduqxv14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1kzpfyl</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Easy French Bling  #ClawsbyRaven  My 15 year old granddaughter!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3j0f2xv9z14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1kzpeej</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>ATLA nails 🌊🪨🔥💨</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cm1clp9ty14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1kzp1l9</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>🖤Hand painted corpse bride nails 🖤</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ghpfkiwu14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1kzp19u</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Trying a new vibe</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fq9e4rtu14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1kzox4g</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I'm not nail artist but I just did ladybugs and I'm very proud of myself</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u78dvgxmt14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1kznxnp</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Next nail set?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptek0tvmj14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1kznovz</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>UV lamps</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kznovz/uv_lamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1kzni51</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>So glad I found my nail tech</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzni51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1kzn9ug</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Happy national nail tech day</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzn9ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1kzn6v8</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Healing My Nails Progress</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzn6v8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1kzmxec</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Obsessed with this glittery pink!!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qvqo96h914f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1kzmumz</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Full Set at Home with Junk Nail</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv973ilr814f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1kzmtuo</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Did my friend’s nails!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzmtuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1kzmpgz</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Accidental Dylan Purple Nails</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzmpgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1kzmk01</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Chocolate covered Strawberry nails</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4h7x9x9t514f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1kzmjvh</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>kicking off neon summer season</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzmjvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1kzmcdb</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Peaches</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzmcdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1kzlx13</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Obsessed with my birthday set 😍</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlne0v2nz04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1kzlvpw</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Nail art for shorties</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vh8yi7az04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1kzl1ln</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Why can you still see the whites of my nails through the polish?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzl1ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1kzlpds</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Floral design inspired by Vietnamese Ao Dai design I saw</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3vx5a4nx04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1kzlevg</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Will I get charged extra for a fill if some of the nails came off?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzlevg/will_i_get_charged_extra_for_a_fill_if_some_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1kzl9nh</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Is nightly cuticle oil enough to moisturize these thirsty bitches?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9xeyp6ht04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1kzky4v</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Attempt at Jolly Rancher strawberry Frenchies</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf8n2yeiq04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1kzky40</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>The thumb is my favorite nail 🥰🐜</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzky40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1kzkt1b</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Ink and Petals 🖤🌸</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vstj8g16p04f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1kzkk3d</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>First attempt at 3D art &amp; press ons</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/829cj170n04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1kzkhh9</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Growth</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzkhh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1kzkavk</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Classic shellac french manicure from a local salon🥰</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3r92vjok04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1kzk7ta</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Today's theme was silver 🩶</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzk7ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1kzk00u</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>How much would these nails cost you where you are?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5diemh0i04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1kzk46g</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uqf9jyvi04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1kzjtep</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>The nail artist‘s freestyle</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1t70s3eg04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1kzjd5a</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>What causes nails to curve/warp like this at sides?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzjd5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1kzjb4w</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>$95 nails and toes. Is this bad?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzjb4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1kzjcib</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>In love with the cat eye look 💗</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgsypu2dc04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1kzj67u</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Website Suggestions</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzj67u/website_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1kziv7a</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Are these ok for beginner gel and nails in general?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kziv7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1kzj4m4</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Working in a salon</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzj4m4/working_in_a_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1kzirgm</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>My nails from my earlier post,</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82xp0gbf704f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1kzhoz6</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzhoz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1kzigmb</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Help me to find</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzigmb/help_me_to_find/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1kzi1xl</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Shorties inspired by this sub! ✨️</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzi1xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1kzhqx1</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Acrylic for strengthing nails???</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzhqx1/acrylic_for_strengthing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1kzhlgk</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Was going for simple summer. I’m in love!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qxysmi0yz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1kzhk4d</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Natural nail art</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5rbayznxz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1kzh7p3</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Yellow 💛</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzh7p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1kzgzae</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>rate my nails from last month</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgnxwf58tz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1kzgv5p</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>My second time using blooming gel and I’m so mesmerized</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzgv5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1kzgtol</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>What type of polish is this?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzgtol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1kzg4u8</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>What Fruit would you have on thumb and pinky?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5mk43tqrmz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1kzg1ek</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Pink Marble</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpwelyr1mz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1kzfxfm</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Starting my big girl job Monday, decided to go classy!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzfxfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1kzftih</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Sister’s graduation nails</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzftih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1kzfq1d</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>DIY Nails. Took 5! Hours</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzfq1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1kzf84w</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Still learning the basics but loving this color!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xel0hvk2gz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1kzf6nn</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>This cateye set before i get my fill tomorrow</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijkbetirfz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1kzeyi9</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Can you use press on nails for one day and remove them easily?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzeyi9/can_you_use_press_on_nails_for_one_day_and_remove/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1kzerj0</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Hibiscus 🌺</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzerj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1kzep2u</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Have you ever washed hands mid full set?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzd9ytm5cz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1kzegnx</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>How I grew my nails and care for them</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4ya1aafaz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1kzej7a</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>My tech did me good</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzej7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1kzee60</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>I peaked on this one hand. The other will forever live in her shadow, because I cannot repeat this with my non-dominant 🥲</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxjd900x9z3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1kze1ui</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Which one’s your favourite??Been a nail technician for 3 months now and here’s my work! ✨</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kze1ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1kze42u</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Rapunzel inspired nails! - done by me</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fldb2xex7z3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1kze8k0</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Loving these new nails</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2h1n5vt8z3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1kzdy5p</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Hit or miss?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4aaurktp6z3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1kzdssd</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>first time getting nail extensions :&gt;</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u94ilwsm5z3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1kzcpnx</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>My more recent set</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1yovrtlxy3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1kzcmgo</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Do they look good or should I go shorter (press on nails)</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzcmgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1kzcd0q</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>new nails !! 🩷💛</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzcd0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1kz9q5k</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Am I overthinking/ overreacting here?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kz9q5k/am_i_overthinking_overreacting_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1kzbzza</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Pokemon Inspired Fluid Art</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzbzza</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1kzc0ro</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>I went a little wild 😅😜</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gf55n9ecsy3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1kzbq70</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Obsessed with these mermaid nails I got yesterday!!! 🧜‍♀️  (and found a friend 🥰🐝)</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzbq70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1kzaikj</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>tips on tips vs builder gel?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzaikj/tips_on_tips_vs_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1kzb48h</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>BIAB question</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzb48h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1kzb1sl</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Doing nails at home goes wrong!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzb1sl/doing_nails_at_home_goes_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1kzb5ak</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Did my mums nails this afternoon ❤</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbsnunj5my3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1kzb3hy</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Press on vs hard gel</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzb3hy/press_on_vs_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1kzay5c</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Decided to complicate my life for the next three weeks</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7lf2ybtky3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1kzan8c</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Ready for pride!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzan8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1kzajd2</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Semi-permanent enamel 😍</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfbkblbthy3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1kzac4k</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Red vs. Purple, which set is your vibe? 💅</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzac4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1kzab03</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Regular polish under a gel top coat.✨</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuosk5b6gy3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1kz9dbu</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>DIY Polygel with Short Square Tips</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz9dbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1kz8vk8</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Overly picky?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/351z3hu56y3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1kz8lqw</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Caboodle Nails</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv0yuni94y3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1kz8jky</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Asked for yellow, orange and pink with a shape seen on @vintage_dusties on insta</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz8jky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1kzrsus</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Do you think these Fancy Gloss shades return at some point?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzrsus</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1kzr6i5</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>My goal mani</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzr6i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1kzp4sz</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>obsessed with my avril lavigne era 🩷🖤✨</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzp4sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1kzoegz</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>💅New Nail Supply Store Grand Opening in Sarasota, FL ✨ Giveaway info✨</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzoegz/new_nail_supply_store_grand_opening_in_sarasota/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1kznk1r</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>My collection thus far</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kznk1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1kzmrhe</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>When Music is your Muse</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jglnit3v714f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1kzmkaa</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>ILNP Aspen in the mountains seemed fitting 🌲⛰️</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wxhepru514f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1kzmgkw</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Goblins and Ghoulies compared to EdM Key Drama and Dam Polish Grave Mistake</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxar4cvv414f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1kzm672</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Next mani advice</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcivyhb2214f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1kzlf49</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Pastel Shimmer Skittle</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzlf49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1kzlbm4</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Any tips?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6q4mfx0u04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1kzkyz8</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Finally purchased more shelves and organized so every bottle has a spot now</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/387zgm3qq04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1kzkw3m</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Hidden Potential</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5lxfzzzp04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1kzkqsd</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>What is this liner?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzkqsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1kzkdov</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Cuticle Work</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdurugzdl04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1kzkcml</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Tis the season for PRIDE 🩷💛🩵</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzkcml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1kzjt4a</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>First time magnetic user, ya’ll were not exaggerating 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxv7oiccg04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1kzjdp7</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>ISO - this color in nail polish!!!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzjdp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1kzjdkm</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Vaporwave + Flower Child 🤩</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzjcqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1kzj6m4</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Bad Week? F*ck this Sh!t</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzj6m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1kziqvk</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>BKL The Chosen One is Chosen for Evil</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/db842f9a704f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1kzij9x</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>This polish is giving me 90s Sanrio vibes and I’m here for it</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzij9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1kzi5ug</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Finally convinced myself not to jump on the new Mooncat release because I had a close enough color already.... only for my bottles to fall off a shelf this morning. RIP.</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tirfw1tw004f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1kzhaye</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Me when Fancy Gloss opened up tonight</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8mjl8kovz3f1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1kzgyze</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>I'd love a holo/magnetic with this pallet</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp1ecf36tz3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1kzgxvr</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Shadow Mommy BKL</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzgxvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1kzgmnx</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>First time post and it’s a neutral color haha</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzgmnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1kzgd75</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Fired Up - Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzgd75</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1kzgbza</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Why might jojoba oil dry out cuticles?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzgbza/why_might_jojoba_oil_dry_out_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1kzgap5</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>🌴 Back with the 80s Miami living room vibes 🦩</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzgap5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1kzgah6</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>If you have Mooncat House of Hades, use a top coat!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzgah6/if_you_have_mooncat_house_of_hades_use_a_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1kzfj74</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Finding your Perfect Red is always so rewarding 🥰</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzfj74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1kzfe1h</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>A color experiment that actually worked!</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wkgreu77hz3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1kzfb9q</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Looking for green suggestions</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzfb9q/looking_for_green_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1kzf7ap</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>What are the most GLOWY polishes in existence?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzf7ap/what_are_the_most_glowy_polishes_in_existence/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1kzf4cu</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Remove gel</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzf4cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1kzev9h</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Onycholysis and biab</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzev9h/onycholysis_and_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1kzeqn2</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Saw someone else post their swatch books so I wanted to join in! This is a result of a year and a half of collecting, basically funneling all of my "fun money" into nail polish 😂</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjjql1zgcz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1kzeoxg</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Solar AND Thermal - I'm in LOVE</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzeoxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1kzemu4</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>New favorite summer-y bright pink!!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzemu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1kze3sd</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>🦋ethereal butterfly wings🦋</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kze3sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1kzdy0s</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>cuticle oil</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzdy0s/cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1kzdvf1</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>All the swatches at once!</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzdvf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1kzcyi0</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Corpse, but chic(?)</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7c8gvo0ezy3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1kzceq7</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Book Club Nails</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sb7ef8fvy3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1kzccqi</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Not the best paint job, but a Happy Springtime mani after not painting my nails for months due to the blahs…</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzccqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1kzc634</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Hopping into a Ribbiting Weekend 🐸</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzc634</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1kzc3at</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Pokemon Inspired Fluid Art</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzc3at</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1kzbwoc</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Last Mani of May</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzbwoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1kzbs5z</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Art Deco</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/Md28Gxn.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1kzbdpg</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Rainbow polish sets?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzbdpg/rainbow_polish_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1kzawmq</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Gothic-core picnic nail art</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzawmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1kz7abq</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>My fave skittles</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz7abq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1kza9z4</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>EDM - what am I missing/what can I remove?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ri8w3qyfy3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1kza26n</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Hummingbird Multi-chrome Skittle</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kza26n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1kz9w4x</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Bee’s Knees ‘spicy’</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pgirwh59dy3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1kz9v2c</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>🌜🌌Night Sky🌌✨️</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz9v2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1kz9pib</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Peony For your Thoughts by LynB</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz9pib</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1kz9l7c</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Get your Knit Together by KbShimmer</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz9l7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1kz9jcd</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>ILNP new release, must haves, and sale question</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kz9jcd/ilnp_new_release_must_haves_and_sale_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1kz8t2a</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Do i have to cut off the damage completely or can i try growing out like this?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2t1lx3o5y3f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1kz8c0y</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Psilo-sibs vs ILNP Illusions?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kz8c0y/psilosibs_vs_ilnp_illusions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1kz7x6i</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Nothing makes me happier than a good chunky glitter</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnyf2s2hzx3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1kz7pvj</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Is this too much?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz7pvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1kz7l8n</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Can I just say WOOOOOW</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz7l8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1kz7aht</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>A rosy flaky! Hertis Rose by Alchemy Lacquer</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz7aht</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1kz7877</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Being canadian</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kz7877/being_canadian/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1kz75oo</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Mooncat - Treachery in the Blue x ILNP - Bluebell</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz75oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1kz6htl</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Orchid Tariffs and this glow are killing me!</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz6htl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1kz6844</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>indie brand recommendations?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kz6844/indie_brand_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1kz645x</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Surprised at this one!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz645x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1kz59um</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>I’ve been painting my own nails since I was 10</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5khz7dedgx3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1kz58y4</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz58y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1kz4tyy</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>First Polished for Days Order</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz4tyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1kz4tq0</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>remedy collection (gifted pr)</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz4tq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1kz34y3</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>ILNP Aussie Group Buy/Swap/Resell Facebook Group</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kz34y3/ilnp_aussie_group_buyswapresell_facebook_group/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1kz2wxg</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>EdM or ILNP is the question 😩</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz2wxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1kz1pwh</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>I'm normally a gel enthusiast but PPU changed my mind about using polish again</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz1pwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1kz1l3x</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>do your nails ever draw blood? 😅 nails looking dangerously good… literally.</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz1l3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1kz0us1</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Y'all!</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz0us1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1kz0q8g</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Cadillacquer - Solar Nebula - absolutely mesmerizing</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gavjxux5bw3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1kyz803</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Loving the BKL Neons</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/elvzg48itv3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1kzpl7c</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Waiting for December to recreate snowflakes ❄️ @isabellanails</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzq0tapw024f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1kzph6t</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>🖤Corpse bride nails</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1gn8henz14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1kzo5cb</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>The first set of press on nails I made.</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t30t3psnl14f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1kzo41d</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Mario nails</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dkcujmbl14f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1kzmntt</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Custom ‘Goth Inspired’ Set 🖤🩶</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnqdsyjv614f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1kzmnet</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>full colors and design what do you think?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lh5yk1r614f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1kzlnq8</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Florers inspired by a floral design I saw on a Vietnamese Ao Dai.</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd5jqcn7x04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1kzkeo0</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Just a quick little color change I was in a rush that’s why you see pop of green lol</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7w0wl1nl04f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1kzk68p</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Ink and Petals 🖤🌸</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j5l1m0fgj04f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1kzizza</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>How to be faster?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhf7jque904f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1kzigzv</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Greek gods inspired nail art for my daughter</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzigzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1kzig51</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Graduation nails for my daughter's girlfriend</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzig51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1kzfvvo</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Love this set ! 5 hours later</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzfvvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1kzfrn3</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Bratz nail art</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j71oa9sqjz3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1kzdytw</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>my first attempt at chrome design</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzdytw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1kzd88n</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Water nails!!</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzd88n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1kzarak</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Ice cream paint job</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b25i0c8ejy3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1kz8hc3</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Best drugstore topcoat for stickers?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kz8hc3/best_drugstore_topcoat_for_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1kz8237</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Finished up my Disney set, so pleased with these!</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz8237</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1kz7fzf</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Rainbow nails 🌈</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kz7fzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1kz4u0l</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>did my fav set on myself in a while &lt;3</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmnyhbf3dx3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1kz4miv</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Nicki Minaj inspired nail art. With 3D elements.</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3s5wgxgbx3f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun  1 08:11:14 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_01.xlsx
+++ b/data/collected_data/2025_06_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1318"/>
+  <dimension ref="A1:C1521"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22839,6 +22839,3457 @@
         </is>
       </c>
     </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1l0jqnq</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Press ons or Nail Salon?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l0jqnq/press_ons_or_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1l0hv93</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Very new to getting nails done and have a few questions!</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l0hv93/very_new_to_getting_nails_done_and_have_a_few/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1l0gzng</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Can I use gel glue as a base coat?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l0gzng/can_i_use_gel_glue_as_a_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1l0gwk3</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Watercolor florals (freehand)</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wq65ghl094f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1l0gs0x</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>natural or fake?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0gs0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1l0gqvb</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Free $8 Code for Chillhouse Nails</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2b316dwwy84f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1l0g8wq</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Thought the first ones were too neon. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0g8wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1l0geb5</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Had to show my newbie DIY builder gel mani 🥹</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0geb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1l0fuco</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Anyone know where i can find a dip powder in this color?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0fuco</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1l0fl3m</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>First time trying juicy nails 🍊</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bu6saajum84f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1l0fa1t</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>First time getting Acrylics; paid $95. Am I over reacting or are these poorly done?</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0fa1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1l0fh40</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Fruit Nails🥭</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d22oamrpl84f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1l0f8ap</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Tie Dye for Pride 🌈</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8yp3aoaj84f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1l0e7vn</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Can't get rubber base or builder gel to stay on</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0e7vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1l0e2t4</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Cuticle Remover</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l0e2t4/cuticle_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1l0dppj</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Rainbow Trout nails 🎣</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0dppj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1l0cy9l</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Birthday set I did on a friend of mine! What do we think?</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0cy9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1l0cx78</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Currently wearing Jelly Filled Fountain by Victorian Varnish</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oe75a6htw74f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1l0crgu</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Cherry for summer!!! 🍒🍒🍒</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0crgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1l0cnil</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Why Do My Nails Have these Brown/Translucent Stains</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0cnil</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1l0cp1e</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>What nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0cp1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1l0cn7r</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>A summertime happiness set</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0cn7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1l0cbfe</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>First time getting acrylics in like 2 years</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0cbfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1l0c94h</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>SCG stickers and acrylic press ons?</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l0c94h/scg_stickers_and_acrylic_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1l0c5up</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Tropical</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hh83bkgip74f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1l0bq1d</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Shiny Rosey Mocha Nails</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0bq1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1l0biah</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>First time doing my own Gel X nails</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cc2o5vsej74f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1l0bdj2</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>polygel on natural nails, used my budgies' molted feathers for this one :)</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0bdj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1l0b8ev</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Best base/activator/top coat for dip nails</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l0b8ev/best_baseactivatortop_coat_for_dip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1l0ard3</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>My favorite color this year!</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy9iyu8vc74f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1l0arci</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>New set - “bubble bath”</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwj1jadvc74f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1l0aiv6</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Tried out a new place, nail tech did not disappoint! 💅🩷</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hldjqp3xa74f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1l0ae7h</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>fresh set 😎</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0ae7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1l0ab3w</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>My nail tech wanted to freestyle 🤩</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0ab3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1l09gw2</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Sky Blue💙</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l09gw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1l09euw</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>I love my nails tech so much 💅🏼😤</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l09euw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1l09dv3</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Obsessed!🍒</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5lk350h174f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1l096yu</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Is this overfilling the cuticle? I have no clue thanks sorry!</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l096yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1l0903g</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Recent Looks 👀</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0903g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1l07ef1</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>What ACRYLIC POWDER will give me this exact color or close as possible</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1oqlrmfl64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1l08aik</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Chrome Nails Video</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gegm3rngs64f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1l08i0w</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw65kf39u64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1l08b9u</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Creamsicle Couture</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibgi10fqs64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1l07tit</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>How to avoid these white spots that appeared the next day?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6irhwx9ro64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1l07sww</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Not sure if this is too red for my skin tone.</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uobe1jgmo64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1l07ou0</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Did this set on my niece, one of my favorites so far!</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l07ou0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1l07hqc</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Creative French 🫶🏻✨️ with animal print</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0u1xryz3m64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1l076dz</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Custom Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ps70r3cnj64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1l06ux9</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Proud 🩷</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97rq2l35h64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1l06pcg</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>What do you think about men’s manicure? It’s my new work 🐾💕</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l06pcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1l06oyl</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Poly gel extension + purple cat eye, how did I do</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l06oyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1l06fe0</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Just got a fill -  but realize now I HATE THE COLOR. Can I simply get a new color?</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l06fe0/just_got_a_fill_but_realize_now_i_hate_the_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1l067mh</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Nails breaking</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwakyilzb64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1l0494j</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Summer sunrise nails</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecjdhtdlw54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1l04bdx</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Chinese styled nails</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l04bdx/chinese_styled_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1l05v24</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Mermaid 🧜🏻‍♀️ Nails</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6z1zdhn8964f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1l05m7r</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>My Emerald Enigma! 💚</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nexv31ka764f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1l05lwk</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>DIY Press ons for flat nails</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l05lwk/diy_press_ons_for_flat_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1l05bhu</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Which shapee</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l05bhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1l059ad</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Nails in gothic style</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l059ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1l04zf6</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Please give me nail advice! 🙏</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l04zf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1l04y91</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Blue pedi</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l04y91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1l04ws7</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>How many salons and techs did you go through before finding someone you stuck with?</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l04ws7/how_many_salons_and_techs_did_you_go_through/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1l04utm</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Thoughts on nail length for an 11 yo</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l04utm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1l04u5m</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Press ons are my jam now!</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/begvxyf4164f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1l04s24</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>fresh nails 💐</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6j318yuo064f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1l04plq</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>❤️ my nail tech!</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5gbnhg6064f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1l04ntf</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>How often do you need to refill?</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l04ntf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1l04ive</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Are my nails to short or long?</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l04ive</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1l04ad3</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>+10 Aura 💅</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l04ad3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1l0415w</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Your favorite top coat?</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0415w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1l037v2</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>the eye of the tiger</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l037v2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1l03425</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Showing off my nails ⋆˙⟡˙⋆</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l03425</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1l02op9</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>New Mani</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5c05e6rk54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1l02iah</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>is getting gel manicures good for very brittle nails?</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l02iah/is_getting_gel_manicures_good_for_very_brittle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1l018dr</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>How would you fix this?</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2vkqkwq954f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1l01i4g</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Beginner Nail Artist…</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vku2ukptb54f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1l01y29</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>watch is sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mb165x07f54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1l01n9s</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Purple 🥰</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j58aaptxc54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1l01fqq</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Buggy asf🐞🐞🐞</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l01fqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1l01f00</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Engagement nails! 🥰</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/haz0rrn5b54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1l01due</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Second set of gel nails I’ve ever done</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hg9alpwa54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1l01ak2</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Chrome Jade?</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l01ak2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1l0196e</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>vintage Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1tg5fyw954f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1l00o2e</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>I loved u/BluLilyx 's nails so much, I used them as inspo for my own - and I think my tech knocked it out of the park.</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l00o2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1kzudkw</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Why do my DIY gel nails split and chip?  🍟</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzudkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1kzwcyc</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Dfk how do i get this stuff off</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzwcyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1l00253</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Anyone know what color this is? 😍💅</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imbceu0v054f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1kzzj2p</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Why is the gel on my pointer and middle finger always lifting?</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwnxawibw44f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1kzzuih</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Had to cut off my natural nails that I've been growing out for 3 months cause one of my nail broke!😭😭</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wy89zua8z44f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1kzx7ks</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>I make my own press on nails and paranoid, is this contact dermatitis?</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a42j24m3e44f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1kzz21h</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Am I crazy?</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o13dn1z7t44f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1kzyk8o</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Nail beds have been flattened and it makes me anxious, will they correct themselves?</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzyk8o/nail_beds_have_been_flattened_and_it_makes_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1kzxq9p</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>can i add polish without filing off</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzxq9p/can_i_add_polish_without_filing_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1kzxnve</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzxnve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1kzw6nq</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Recent Manicure and Pedicure</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzw6nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1kzvnbc</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>What are some safety gloves for short almond nails?</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kzvnbc/what_are_some_safety_gloves_for_short_almond_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1kzu7ew</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>What can you say about this set?</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzu7ew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1kztdit</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>what are these dents on my nails?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kztdit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1kzsoaj</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Starting my natural nail journey!</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzsoaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1l0jq9y</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Neat and Tidy</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0jq9y/neat_and_tidy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1l0j57a</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>love yellow but boy are they hard to. work with</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhryofc9q94f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1l0j15p</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>I want cute nails but have allergies, please help</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0j15p/i_want_cute_nails_but_have_allergies_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1l0imzc</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Jade Greens!</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bf2ibfnck94f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1l0impb</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>May mani roundup :)</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0impb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1l0i4vz</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Goodbye, Muppet*Vision 3-D</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0i4vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1l0gzlj</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Nails won’t dry, gel or regular polish</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0gzlj/nails_wont_dry_gel_or_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1l0grle</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>May Manis</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0grle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1l0ghxi</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Which nail brand polish doesn’t suits with your body chemistry?</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0ghxi/which_nail_brand_polish_doesnt_suits_with_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1l0gggd</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>First KB Shimmer order!!!</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0gggd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1l0g9wl</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Cracked No Shrubs vs Cirque Kelly Jelly swatch?</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0g9wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1l0g9qu</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Looking for</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0g9qu/looking_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1l0fmrk</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Looking for a Chanel Cruise dupe</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zst7umbn84f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1l0euoj</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Pretty in pink to end May flowers</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0euoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1l0erp2</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>My nails are in terrible shape. I’m getting married in two weeks. Would gel or acrylics be appropriate?</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovj5k8wte84f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1l0ekvw</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Lacqueristas, I will boldly claim this is the best red creme polish ever created</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am2yf0yzc84f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1l0e5p6</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>ILNP ROSEWATER</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z7wly49w884f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1l0dez6</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>My favorite Mani this month</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0dez6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1l0d1df</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Jelly polish not working with silicone nail stamper</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0d1df/jelly_polish_not_working_with_silicone_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1l05omt</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>My fault or the salons?</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l05omt/my_fault_or_the_salons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1l07z8o</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Hello from the Dominican Republic!!!!</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l07z8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1l0c3yv</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Okay, I See You, Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0c3yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1l0by8x</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>My partner let me do his nails!</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9sjmdbjn74f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1l0bqzq</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Did nail art for the first time… Now I have no pinkie nail.</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0bqzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1l0bo5b</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Mystic Dust and Divination</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0bo5b/fancy_gloss_mystic_dust_and_divination/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1l0avjz</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Currently wearing Jelly Filled Fountain by Victorian Varnish 😍</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sfvzxw1vd74f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1l0a438</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>What are your MUST HAVE ILNP polishes?</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0a438/what_are_your_must_have_ilnp_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1l09z2p</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Seaglass nails 🪸</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l09z2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1l09vtf</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>thermal nail polish 💜🩷</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t1fnd52m574f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1l09s5y</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>First impression: mooncat's green-eyed-monster</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/86ihdzhr474f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1l09j6o</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Lola Belle Yellow Love</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l09j6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1l09g9d</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>What brought you to the world of lacquers?</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l09g9d/what_brought_you_to_the_world_of_lacquers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1l0997y</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>True lime green!</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l0997y/true_lime_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1l0961u</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>The beautiful shiftinnes of ILNP's Orbit</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wlfnwyo8y64f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1l095gl</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>cuticles vs proximal nail folds</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jla7pewjz64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1l094lw</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Why does this routine work?</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yczgurccz64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1l084ab</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>What are your favorite metallics?</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l084ab/what_are_your_favorite_metallics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1l082s6</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Looking for the OPI (or possibly Orly ?) Olive polish that someone posted recently. I DID search, but I think the post may have been removed. Does anyone remember the name, please? I would really like to purchase. TIA</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l082s6/looking_for_the_opi_or_possibly_orly_olive_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1l07f06</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Same shade?</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l07f06/same_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1l07710</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Swatch comparison please</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke2bpsftj64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1l076cs</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Question about oil soaking</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l076cs/question_about_oil_soaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1l06yk9</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>[ISO] Swatches of Atomic Sour Apple Rings VS. Thorium (Th)</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l06yk9/iso_swatches_of_atomic_sour_apple_rings_vs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1l06kzv</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>DAE pick up Feelin’ Froggy by Painted Polish in May’s PPU?</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8ns4ukxe64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1l06bnr</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Thank you to my bf (now fiance) for proposing when my nails were done with one of my fave polishes!</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwhco1wuc64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1l05yse</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Arara Azul</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l05yse</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1l05af8</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Liquid Fire 🔥</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l05af8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1l051k0</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>May Manis</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l051k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1l04wdj</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Questions about Fancy Gloss Rock Serpent</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l04wdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1l04voo</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>my first ILNP order. any recs?</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2vc8tog164f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1l04kw7</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>My gran passed away a month ago today, and she left me her polish collection. This colour, however??? 😭</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mjf7et3z54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1l038rc</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>First (and definitely not last) time trying watermarbling! 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l038rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1l037wc</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Joie de Vivre in motion🌿💚</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3oizfj5po54f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1l033qh</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>My nails but better</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l033qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1l0337h</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>My husband does my nail art - strawberry edition</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xpzzvvyk54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1l02zu0</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Are any detectives in here able to deduce what polish Taylor Swift is wearing in her most recent photos lol?</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imollg82n54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1l014oq</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>First post!</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0exxczx854f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1l02e0f</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>May manis 💐💅🏼</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l02e0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1l01wg1</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Essie’s Frosted Fantasy over red and black :)</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l01wg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1l01uv3</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Get that dopamine ✨ sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kl2g1bz9d54f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1l01uo9</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>French tips</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ogr9kbehe54f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1l01qzp</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Should I go squoval or keep round?</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l01qzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1l01c0v</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>DIY Magnetic Topper</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uuvc5q0ja54f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1l00ty5</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Starrily nothern Lights</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l00ty5/starrily_nothern_lights/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1l00ghw</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>PSA: Fancy Gloss makes gorgeous thermals- here's Once in a Purple Moon</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l00ghw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1l00fzn</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Blue Jeans-Salon Perfect🩵</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l00fzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1l000tm</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Help me with my ILNP cart</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l000tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1kzzyk0</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>What in the budget supermarket wizardry?</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzzyk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1kzzlcc</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Finally: a polish that actually live up to its swatches.</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzzlcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1kzyzhp</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Where to buy Lurid</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzyzhp/where_to_buy_lurid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1kzyz2a</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>LA Girl Holographic Top Coat</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzyz2a/la_girl_holographic_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1kzys9k</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>Kendrick Lamar GNX inspired mani for his SF show</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyfply33r44f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1kzyi41</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>BKL I am an appetite</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzyi41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1kzyav5</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>May Manis 💐</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzyav5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1kzy9ak</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>Eye searing 🌈recs</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzy9ak/eye_searing_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1kzxxj5</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Emeralds on my fingers</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzxxj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1kzxq8d</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Essie Gel Couture TC is that girl</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5wd02kgi44f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1kzxc8v</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>Sharing my first good quality nail polish order 🥳 (ILNP)</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzxc8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1kzwzw4</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>First ILNP haul</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxpstuzac44f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1kzwt4c</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>frogs.</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpqxywooa44f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1kzwnkk</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Chrome powder over regular polish</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouz3y98a944f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1kzuzai</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Joie de Vivre 2.0🌿</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzuzai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1kzaws1</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>Overfiled my nails and in recovery mode. Can I use normal polish over them while they heal?</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzaws1/overfiled_my_nails_and_in_recovery_mode_can_i_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1kzdzue</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>Confused about OPI Nail envy…?</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzdzue/confused_about_opi_nail_envy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1kzenjh</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>similar shades??</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzenjh/similar_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1kzeww2</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Orly Morning Dew 🩵</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzeww2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1kzsqf8</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>White with gold ombr tips for my wedding! This might be my favorite manicure Ive ever had.</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/gUNCeul.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1kzt20e</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>Polishes like mooncat mermaid bait?</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzt20e/polishes_like_mooncat_mermaid_bait/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1kzsvdu</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>May nails 🌸🌺💅</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzsvdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1kzs2c4</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>Dupe for Discontinued Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzs2c4/dupe_for_discontinued_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1kzrzqp</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>Help with nail bed shape!</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kzrzqp/help_with_nail_bed_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1l0fivm</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>Spirited Away Nails</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0fivm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1l0dtru</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>The Stardew Valley sub loved these, so I figured y’all might like them too!</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l0dtru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1l0bw91</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>some grad nails i did for a family friend 🤩💅🏻</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edyz5lg0n74f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1l08mfs</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>Holo chrome and rainbow blobs</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l08mfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1l08g8s</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>Custom Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezajwqjtt64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1l07c55</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>Space Bees 🐝</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/013i04dxk64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1l06nhu</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>Creamsicle Couture</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9yynyshf64f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1l04vpx</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>Blue pedi</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l04vpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>1l02qlu</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>a little girly pop butterfly set 💖</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l02qlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>1l00uyo</t>
+        </is>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>vacation set</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l00uyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>1l00tf9</t>
+        </is>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>Reverse Fishies</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l00tf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>1kzx2jw</t>
+        </is>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Aquarium Nails, how?</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kzx2jw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>1kzsy3e</t>
+        </is>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>Hand painted nail art. Gel overlay.</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x77g5hme534f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>